<commit_message>
change database to superbase and push test adjust excel ---  add booking date search
</commit_message>
<xml_diff>
--- a/static/templates/motorbike_template.xlsx
+++ b/static/templates/motorbike_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Work_Freelance\Tour\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1CE78A-4C48-4A57-A5DB-09F3A23BEA0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A948B6-825F-462E-BC79-43B4EAFECFE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8868" xr2:uid="{492F029A-8E98-4A79-9B77-CF9AB15A96C9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>ORIGINAL</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>STAFF</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>STATUS</t>
@@ -103,7 +100,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12">
@@ -200,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -320,12 +318,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -343,12 +372,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -376,27 +399,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,6 +414,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,11 +438,44 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -747,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F97E37-B014-4C99-B27C-6BC54D2AD0E2}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C28" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -765,29 +812,29 @@
   <sheetData>
     <row r="1" spans="1:11" ht="8.25" customHeight="1"/>
     <row r="2" spans="1:11" ht="21" customHeight="1">
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="34"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:11" ht="12" customHeight="1">
-      <c r="D3" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="D3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="12" customHeight="1">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="25"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="3.75" customHeight="1"/>
     <row r="6" spans="1:11">
@@ -797,22 +844,23 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="35"/>
+      <c r="G6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="26"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" ht="17.25" customHeight="1">
       <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="27"/>
+        <v>17</v>
+      </c>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -822,12 +870,12 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="27"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -843,192 +891,200 @@
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="G12" s="30" t="s">
         <v>2</v>
       </c>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="J13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15">
+      <c r="B14" s="16"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" ht="15">
+      <c r="B15" s="16"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="38"/>
+    </row>
+    <row r="16" spans="1:11" ht="15">
+      <c r="B16" s="16"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="1:10" ht="15">
+      <c r="B17" s="16"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="1:10" ht="15">
+      <c r="B18" s="16"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" customHeight="1">
+      <c r="B19" s="23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" ht="15">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:10" ht="15">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" ht="15">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1">
-      <c r="B19" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="19"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="39"/>
     </row>
     <row r="20" spans="1:10" ht="15">
       <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="20"/>
+      <c r="H20" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
+      <c r="E23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
       <c r="J23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="24" spans="1:10">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+    </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="17"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
     <row r="27" spans="1:10" ht="20.25" customHeight="1">
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="34"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="D28" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
+      <c r="D28" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="G30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="4"/>
+      <c r="G30" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="41"/>
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="2"/>
       <c r="B31" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1038,12 +1094,12 @@
     </row>
     <row r="32" spans="1:10" ht="15">
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15">
       <c r="B33" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1062,193 +1118,217 @@
       <c r="B35" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C35" s="41"/>
     </row>
     <row r="36" spans="1:10">
       <c r="B36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="C36" s="30"/>
+      <c r="D36" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="G36" s="30" t="s">
         <v>2</v>
       </c>
+      <c r="H36" s="30"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="B37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="J37" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="13.5" customHeight="1">
+      <c r="B38" s="16"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="38"/>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1">
+      <c r="B39" s="16"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1">
+      <c r="B40" s="16"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="41" spans="1:10" ht="15">
+      <c r="B41" s="16"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="38"/>
+    </row>
+    <row r="42" spans="1:10" ht="15">
+      <c r="B42" s="16"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="38"/>
+    </row>
+    <row r="43" spans="1:10" ht="15">
+      <c r="B43" s="23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="13.5" customHeight="1">
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:10" ht="15" customHeight="1">
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="1:10" ht="14.25" customHeight="1">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:10" ht="15">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:10" ht="15">
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="18"/>
-    </row>
-    <row r="43" spans="1:10" ht="15">
-      <c r="B43" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="19"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="B44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I44" s="29"/>
-      <c r="J44" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="24"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
       <c r="B45" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="J46" s="15"/>
+      <c r="J46" s="13"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
+      <c r="E47" s="13"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
       <c r="J47" s="3" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="48" spans="1:10">
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+    </row>
     <row r="49" spans="2:10" ht="22.5" customHeight="1"/>
     <row r="55" spans="2:10">
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="E58" s="15"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="E58" s="13"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="26">
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="H44:I44"/>
     <mergeCell ref="B43:I43"/>
@@ -1260,6 +1340,7 @@
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Dockerfile with LibreOffice for PDF generation--adjust excel
</commit_message>
<xml_diff>
--- a/static/templates/motorbike_template.xlsx
+++ b/static/templates/motorbike_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00.Work_Freelance\Tour\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A948B6-825F-462E-BC79-43B4EAFECFE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B1E581-9143-4C91-A05F-A1DDF8173EE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8868" xr2:uid="{492F029A-8E98-4A79-9B77-CF9AB15A96C9}"/>
   </bookViews>
@@ -100,8 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12">
@@ -354,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -372,12 +371,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -399,12 +392,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,70 +399,85 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -794,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F97E37-B014-4C99-B27C-6BC54D2AD0E2}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48:I48"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -812,29 +814,29 @@
   <sheetData>
     <row r="1" spans="1:11" ht="8.25" customHeight="1"/>
     <row r="2" spans="1:11" ht="21" customHeight="1">
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:11" ht="12" customHeight="1">
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:11" ht="12" customHeight="1">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="18"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" ht="3.75" customHeight="1"/>
     <row r="6" spans="1:11">
@@ -844,19 +846,19 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="41"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="18"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="19"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="17.25" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
@@ -870,7 +872,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="20"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1">
       <c r="A9" s="2"/>
@@ -891,37 +893,37 @@
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="41"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="G12" s="30" t="s">
+      <c r="E12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="30"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="26" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="23"/>
+      <c r="I13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -929,82 +931,87 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="B14" s="16"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="38"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="B15" s="16"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="38"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:11" ht="15">
-      <c r="B16" s="16"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="38"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:10" ht="15">
-      <c r="B17" s="16"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="38"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="15">
-      <c r="B18" s="16"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="24"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
       <c r="J19" s="39"/>
     </row>
     <row r="20" spans="1:10" ht="15">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="40"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="41"/>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" s="3" t="s">
@@ -1015,71 +1022,71 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="E23" s="11"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="15"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
     </row>
     <row r="27" spans="1:10" ht="20.25" customHeight="1">
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="22"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="29"/>
-      <c r="I30" s="41"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="2"/>
@@ -1118,37 +1125,37 @@
       <c r="B35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="41"/>
+      <c r="C35" s="18"/>
     </row>
     <row r="36" spans="1:10">
       <c r="B36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30" t="s">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="30"/>
-      <c r="G36" s="30" t="s">
+      <c r="E36" s="17"/>
+      <c r="G36" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="30"/>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="B37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="26" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="27"/>
-      <c r="I37" s="9" t="s">
+      <c r="H37" s="23"/>
+      <c r="I37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="J37" s="6" t="s">
@@ -1156,86 +1163,87 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="13.5" customHeight="1">
-      <c r="B38" s="16"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="38"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
-      <c r="B39" s="16"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="38"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1">
-      <c r="B40" s="16"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="38"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="B41" s="16"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="38"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="31"/>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="B42" s="16"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="38"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" ht="15">
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="24"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="38"/>
       <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" ht="15">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="23" t="s">
+      <c r="C44" s="40"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I44" s="24"/>
-      <c r="J44" s="40"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
       <c r="B45" s="3" t="s">
@@ -1246,85 +1254,75 @@
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="J46" s="13"/>
+      <c r="J46" s="11"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
+      <c r="E47" s="11"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
       <c r="J47" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
     </row>
     <row r="49" spans="2:10" ht="22.5" customHeight="1"/>
     <row r="55" spans="2:10">
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="E58" s="13"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="E58" s="11"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G30:H30"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="B24:C24"/>
@@ -1341,6 +1339,16 @@
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>